<commit_message>
corrected labels in the raw data
</commit_message>
<xml_diff>
--- a/usecases/MinimumWorkingExample/Data/Mischungen/2018_04_19_Brecht SVB.xlsx
+++ b/usecases/MinimumWorkingExample/Data/Mischungen/2018_04_19_Brecht SVB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\03_Pruefungen\01_Technologie\05_Beton und Mörtel\BAM 7.3\Brecht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afriemel\Documents\GithubMC\usecases\MinimumWorkingExample\Data\Mischungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93488C9-827C-40FF-A25B-ED9276F087E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25245" yWindow="30" windowWidth="18705" windowHeight="12240" activeTab="2"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sieblinie" sheetId="1" r:id="rId1"/>
@@ -21,12 +22,23 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Rezeptur!$A$1:$K$48</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sieblinie!$A$1:$L$55</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="169">
   <si>
     <t>Kornzusammensetzung von Zuschlaggemischen für Beton</t>
   </si>
@@ -542,11 +554,14 @@
   <si>
     <t xml:space="preserve">  Setzfließmaß in mm</t>
   </si>
+  <si>
+    <t>Zusatzstoff</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
@@ -2254,12 +2269,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2299,33 +2347,6 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2365,18 +2386,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Euro" xfId="3"/>
+    <cellStyle name="Euro" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="2"/>
+    <cellStyle name="Standard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -5025,26 +5040,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" customWidth="1"/>
-    <col min="7" max="11" width="6.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="5" width="6.44140625" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" customWidth="1"/>
+    <col min="7" max="11" width="6.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="277" t="s">
+    <row r="1" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="279" t="s">
         <v>146</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -5071,8 +5086,8 @@
       <c r="Q1" s="48"/>
       <c r="R1" s="48"/>
     </row>
-    <row r="2" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="278"/>
+    <row r="2" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="280"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -5097,7 +5112,7 @@
       <c r="Q2" s="48"/>
       <c r="R2" s="48"/>
     </row>
-    <row r="3" spans="1:18" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="46"/>
       <c r="C3" s="46"/>
@@ -5117,7 +5132,7 @@
       <c r="Q3" s="48"/>
       <c r="R3" s="48"/>
     </row>
-    <row r="4" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>4</v>
       </c>
@@ -5143,7 +5158,7 @@
       <c r="Q4" s="48"/>
       <c r="R4" s="48"/>
     </row>
-    <row r="5" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>5</v>
       </c>
@@ -5171,7 +5186,7 @@
       <c r="Q5" s="48"/>
       <c r="R5" s="48"/>
     </row>
-    <row r="6" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>7</v>
       </c>
@@ -5199,7 +5214,7 @@
       <c r="Q6" s="48"/>
       <c r="R6" s="48"/>
     </row>
-    <row r="7" spans="1:18" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="46"/>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
@@ -5219,7 +5234,7 @@
       <c r="Q7" s="48"/>
       <c r="R7" s="48"/>
     </row>
-    <row r="8" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="188" t="s">
         <v>9</v>
       </c>
@@ -5248,7 +5263,7 @@
       <c r="Q8" s="48"/>
       <c r="R8" s="48"/>
     </row>
-    <row r="9" spans="1:18" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="46"/>
       <c r="B9" s="46"/>
       <c r="C9" s="46"/>
@@ -5268,7 +5283,7 @@
       <c r="Q9" s="48"/>
       <c r="R9" s="48"/>
     </row>
-    <row r="10" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="231" t="s">
         <v>12</v>
       </c>
@@ -5294,7 +5309,7 @@
       <c r="Q10" s="48"/>
       <c r="R10" s="48"/>
     </row>
-    <row r="11" spans="1:18" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="235" t="s">
         <v>15</v>
       </c>
@@ -5334,7 +5349,7 @@
       <c r="Q11" s="48"/>
       <c r="R11" s="48"/>
     </row>
-    <row r="12" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="239" t="s">
         <v>17</v>
       </c>
@@ -5374,7 +5389,7 @@
       <c r="Q12" s="48"/>
       <c r="R12" s="48"/>
     </row>
-    <row r="13" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="239" t="s">
         <v>19</v>
       </c>
@@ -5414,7 +5429,7 @@
       <c r="Q13" s="48"/>
       <c r="R13" s="48"/>
     </row>
-    <row r="14" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="239" t="s">
         <v>20</v>
       </c>
@@ -5454,7 +5469,7 @@
       <c r="Q14" s="48"/>
       <c r="R14" s="48"/>
     </row>
-    <row r="15" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="239" t="s">
         <v>21</v>
       </c>
@@ -5494,7 +5509,7 @@
       <c r="Q15" s="48"/>
       <c r="R15" s="48"/>
     </row>
-    <row r="16" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="239" t="s">
         <v>22</v>
       </c>
@@ -5534,7 +5549,7 @@
       <c r="Q16" s="48"/>
       <c r="R16" s="48"/>
     </row>
-    <row r="17" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="239" t="s">
         <v>129</v>
       </c>
@@ -5574,7 +5589,7 @@
       <c r="Q17" s="48"/>
       <c r="R17" s="48"/>
     </row>
-    <row r="18" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="239" t="s">
         <v>23</v>
       </c>
@@ -5614,7 +5629,7 @@
       <c r="Q18" s="48"/>
       <c r="R18" s="48"/>
     </row>
-    <row r="19" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="235"/>
       <c r="B19" s="236"/>
       <c r="C19" s="237"/>
@@ -5634,7 +5649,7 @@
       <c r="Q19" s="48"/>
       <c r="R19" s="48"/>
     </row>
-    <row r="20" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="148"/>
       <c r="B20" s="148"/>
       <c r="C20" s="148"/>
@@ -5654,7 +5669,7 @@
       <c r="Q20" s="48"/>
       <c r="R20" s="48"/>
     </row>
-    <row r="21" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="249" t="s">
         <v>24</v>
       </c>
@@ -5676,7 +5691,7 @@
       <c r="Q21" s="48"/>
       <c r="R21" s="48"/>
     </row>
-    <row r="22" spans="1:18" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="148"/>
       <c r="B22" s="148"/>
       <c r="C22" s="148"/>
@@ -5696,7 +5711,7 @@
       <c r="Q22" s="48"/>
       <c r="R22" s="48"/>
     </row>
-    <row r="23" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="148" t="s">
         <v>25</v>
       </c>
@@ -5737,7 +5752,7 @@
       <c r="Q23" s="48"/>
       <c r="R23" s="48"/>
     </row>
-    <row r="24" spans="1:18" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="148"/>
       <c r="B24" s="148"/>
       <c r="C24" s="148"/>
@@ -5757,7 +5772,7 @@
       <c r="Q24" s="48"/>
       <c r="R24" s="48"/>
     </row>
-    <row r="25" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="54" t="s">
         <v>12</v>
       </c>
@@ -5783,7 +5798,7 @@
       <c r="Q25" s="48"/>
       <c r="R25" s="48"/>
     </row>
-    <row r="26" spans="1:18" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="252" t="s">
         <v>15</v>
       </c>
@@ -5835,7 +5850,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="239" t="s">
         <v>35</v>
       </c>
@@ -5895,7 +5910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="239" t="s">
         <v>19</v>
       </c>
@@ -5956,7 +5971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="239" t="s">
         <v>36</v>
       </c>
@@ -6017,7 +6032,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="239" t="s">
         <v>37</v>
       </c>
@@ -6078,7 +6093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="239" t="s">
         <v>38</v>
       </c>
@@ -6139,7 +6154,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="239" t="s">
         <v>130</v>
       </c>
@@ -6200,7 +6215,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="239" t="s">
         <v>39</v>
       </c>
@@ -6261,7 +6276,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="235"/>
       <c r="B34" s="236"/>
       <c r="C34" s="257"/>
@@ -6318,7 +6333,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="197" t="s">
         <v>30</v>
       </c>
@@ -6370,7 +6385,7 @@
       <c r="Q35" s="48"/>
       <c r="R35" s="48"/>
     </row>
-    <row r="36" spans="1:18" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="262" t="s">
         <v>40</v>
       </c>
@@ -6419,7 +6434,7 @@
       <c r="Q36" s="48"/>
       <c r="R36" s="48"/>
     </row>
-    <row r="37" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -6433,16 +6448,16 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="O41" s="5"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="O45" s="5"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="20"/>
       <c r="B59" s="32"/>
       <c r="C59" s="21">
@@ -6471,7 +6486,7 @@
       </c>
       <c r="K59" s="9"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="28" t="s">
         <v>125</v>
       </c>
@@ -6509,7 +6524,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="28" t="s">
         <v>126</v>
       </c>
@@ -6547,7 +6562,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="28"/>
       <c r="B62" s="29"/>
       <c r="C62" s="26"/>
@@ -6559,7 +6574,7 @@
       <c r="I62" s="26"/>
       <c r="J62" s="26"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="28" t="s">
         <v>127</v>
       </c>
@@ -6597,7 +6612,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="30" t="s">
         <v>128</v>
       </c>
@@ -6651,26 +6666,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" customWidth="1"/>
-    <col min="8" max="10" width="6.7109375" customWidth="1"/>
+    <col min="3" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" customWidth="1"/>
+    <col min="8" max="10" width="6.6640625" customWidth="1"/>
     <col min="11" max="11" width="8" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="277" t="str">
+    <row r="1" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="279" t="str">
         <f>Sieblinie!A1</f>
         <v>BAM
 7.4</v>
@@ -6693,8 +6708,8 @@
       </c>
       <c r="K1" s="172"/>
     </row>
-    <row r="2" spans="1:11" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="278"/>
+    <row r="2" spans="1:11" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="280"/>
       <c r="B2" s="173"/>
       <c r="C2" s="173"/>
       <c r="D2" s="173"/>
@@ -6711,7 +6726,7 @@
         <v>Haamkens</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="46"/>
       <c r="C3" s="46"/>
@@ -6724,7 +6739,7 @@
       <c r="J3" s="46"/>
       <c r="K3" s="46"/>
     </row>
-    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>4</v>
       </c>
@@ -6742,7 +6757,7 @@
       <c r="J4" s="49"/>
       <c r="K4" s="49"/>
     </row>
-    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>5</v>
       </c>
@@ -6760,7 +6775,7 @@
       <c r="J5" s="49"/>
       <c r="K5" s="49"/>
     </row>
-    <row r="6" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>45</v>
       </c>
@@ -6786,7 +6801,7 @@
       <c r="J6" s="49"/>
       <c r="K6" s="49"/>
     </row>
-    <row r="7" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="47"/>
       <c r="C7" s="47"/>
@@ -6799,7 +6814,7 @@
       <c r="J7" s="47"/>
       <c r="K7" s="47"/>
     </row>
-    <row r="8" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>103</v>
       </c>
@@ -6817,7 +6832,7 @@
       <c r="J8" s="49"/>
       <c r="K8" s="49"/>
     </row>
-    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="178" t="s">
         <v>141</v>
       </c>
@@ -6844,7 +6859,7 @@
       <c r="J9" s="49"/>
       <c r="K9" s="49"/>
     </row>
-    <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>105</v>
       </c>
@@ -6867,7 +6882,7 @@
       <c r="J10" s="49"/>
       <c r="K10" s="49"/>
     </row>
-    <row r="11" spans="1:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="46"/>
       <c r="B11" s="46"/>
       <c r="C11" s="46"/>
@@ -6880,7 +6895,7 @@
       <c r="J11" s="46"/>
       <c r="K11" s="46"/>
     </row>
-    <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="188" t="s">
         <v>107</v>
       </c>
@@ -6900,7 +6915,7 @@
       <c r="J12" s="46"/>
       <c r="K12" s="46"/>
     </row>
-    <row r="13" spans="1:11" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="46"/>
       <c r="B13" s="46"/>
       <c r="C13" s="46"/>
@@ -6913,7 +6928,7 @@
       <c r="J13" s="46"/>
       <c r="K13" s="46"/>
     </row>
-    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="170" t="s">
         <v>108</v>
       </c>
@@ -6946,7 +6961,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="141" t="s">
         <v>110</v>
       </c>
@@ -6988,7 +7003,7 @@
         <v>3.8810000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46"/>
       <c r="B16" s="46"/>
       <c r="C16" s="46"/>
@@ -7001,7 +7016,7 @@
       <c r="J16" s="46"/>
       <c r="K16" s="46"/>
     </row>
-    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="188" t="s">
         <v>111</v>
       </c>
@@ -7016,7 +7031,7 @@
       <c r="J17" s="46"/>
       <c r="K17" s="46"/>
     </row>
-    <row r="18" spans="1:13" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="46"/>
       <c r="B18" s="46"/>
       <c r="C18" s="46"/>
@@ -7029,7 +7044,7 @@
       <c r="J18" s="46"/>
       <c r="K18" s="46"/>
     </row>
-    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="54" t="s">
         <v>48</v>
       </c>
@@ -7052,7 +7067,7 @@
       <c r="J19" s="56"/>
       <c r="K19" s="55"/>
     </row>
-    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="70"/>
       <c r="B20" s="66"/>
       <c r="C20" s="71"/>
@@ -7067,7 +7082,7 @@
       <c r="J20" s="198"/>
       <c r="K20" s="199"/>
     </row>
-    <row r="21" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="141"/>
       <c r="B21" s="142"/>
       <c r="C21" s="44" t="s">
@@ -7088,11 +7103,11 @@
       <c r="J21" s="44"/>
       <c r="K21" s="45"/>
     </row>
-    <row r="22" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="285" t="s">
+    <row r="22" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="296" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="286"/>
+      <c r="B22" s="297"/>
       <c r="C22" s="79">
         <v>300</v>
       </c>
@@ -7112,7 +7127,7 @@
       <c r="J22" s="36"/>
       <c r="K22" s="37"/>
     </row>
-    <row r="23" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="70" t="s">
         <v>62</v>
       </c>
@@ -7130,11 +7145,11 @@
         <v>180</v>
       </c>
       <c r="H23" s="203"/>
-      <c r="I23" s="295"/>
-      <c r="J23" s="296"/>
-      <c r="K23" s="297"/>
-    </row>
-    <row r="24" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I23" s="284"/>
+      <c r="J23" s="285"/>
+      <c r="K23" s="286"/>
+    </row>
+    <row r="24" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="s">
         <v>64</v>
       </c>
@@ -7151,11 +7166,11 @@
         <v>65</v>
       </c>
       <c r="H24" s="203"/>
-      <c r="I24" s="295"/>
-      <c r="J24" s="296"/>
-      <c r="K24" s="297"/>
-    </row>
-    <row r="25" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I24" s="284"/>
+      <c r="J24" s="285"/>
+      <c r="K24" s="286"/>
+    </row>
+    <row r="25" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="70" t="s">
         <v>67</v>
       </c>
@@ -7172,15 +7187,17 @@
         <v>20</v>
       </c>
       <c r="H25" s="203"/>
-      <c r="I25" s="295"/>
-      <c r="J25" s="296"/>
-      <c r="K25" s="297"/>
-    </row>
-    <row r="26" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I25" s="284"/>
+      <c r="J25" s="285"/>
+      <c r="K25" s="286"/>
+    </row>
+    <row r="26" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="70" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="B26" s="66"/>
       <c r="C26" s="90">
         <v>301</v>
       </c>
@@ -7194,13 +7211,13 @@
         <v>110.1</v>
       </c>
       <c r="H26" s="203"/>
-      <c r="I26" s="282" t="s">
+      <c r="I26" s="293" t="s">
         <v>137</v>
       </c>
-      <c r="J26" s="283"/>
-      <c r="K26" s="284"/>
-    </row>
-    <row r="27" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J26" s="294"/>
+      <c r="K26" s="295"/>
+    </row>
+    <row r="27" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="70" t="s">
         <v>117</v>
       </c>
@@ -7219,17 +7236,17 @@
         <v>8.1</v>
       </c>
       <c r="H27" s="203"/>
-      <c r="I27" s="289" t="s">
+      <c r="I27" s="300" t="s">
         <v>165</v>
       </c>
-      <c r="J27" s="290"/>
-      <c r="K27" s="291"/>
-    </row>
-    <row r="28" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="287" t="s">
+      <c r="J27" s="301"/>
+      <c r="K27" s="302"/>
+    </row>
+    <row r="28" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="298" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="288"/>
+      <c r="B28" s="299"/>
       <c r="C28" s="79"/>
       <c r="D28" s="72"/>
       <c r="E28" s="204" t="s">
@@ -7241,11 +7258,11 @@
         <v>414.20000000000005</v>
       </c>
       <c r="H28" s="203"/>
-      <c r="I28" s="295"/>
-      <c r="J28" s="296"/>
-      <c r="K28" s="297"/>
-    </row>
-    <row r="29" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I28" s="284"/>
+      <c r="J28" s="285"/>
+      <c r="K28" s="286"/>
+    </row>
+    <row r="29" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="104" t="s">
         <v>73</v>
       </c>
@@ -7266,11 +7283,11 @@
       <c r="H29" s="209" t="s">
         <v>118</v>
       </c>
-      <c r="I29" s="295"/>
-      <c r="J29" s="296"/>
-      <c r="K29" s="297"/>
-    </row>
-    <row r="30" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I29" s="284"/>
+      <c r="J29" s="285"/>
+      <c r="K29" s="286"/>
+    </row>
+    <row r="30" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="210" t="s">
         <v>76</v>
       </c>
@@ -7292,14 +7309,14 @@
         <f>Sieblinie!D27</f>
         <v>0</v>
       </c>
-      <c r="I30" s="279" t="str">
+      <c r="I30" s="290" t="str">
         <f>Sieblinie!L12</f>
         <v>Quarz</v>
       </c>
-      <c r="J30" s="280"/>
-      <c r="K30" s="281"/>
-    </row>
-    <row r="31" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J30" s="291"/>
+      <c r="K30" s="292"/>
+    </row>
+    <row r="31" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="210" t="s">
         <v>77</v>
       </c>
@@ -7321,14 +7338,14 @@
         <f>Sieblinie!C28</f>
         <v>20</v>
       </c>
-      <c r="I31" s="279" t="str">
+      <c r="I31" s="290" t="str">
         <f>Sieblinie!L13</f>
         <v>Okrilla</v>
       </c>
-      <c r="J31" s="280"/>
-      <c r="K31" s="281"/>
-    </row>
-    <row r="32" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J31" s="291"/>
+      <c r="K31" s="292"/>
+    </row>
+    <row r="32" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="210" t="s">
         <v>119</v>
       </c>
@@ -7350,15 +7367,15 @@
         <f>Sieblinie!C29</f>
         <v>11.5</v>
       </c>
-      <c r="I32" s="279" t="str">
+      <c r="I32" s="290" t="str">
         <f>Sieblinie!L14</f>
         <v>Okrilla</v>
       </c>
-      <c r="J32" s="280"/>
-      <c r="K32" s="281"/>
+      <c r="J32" s="291"/>
+      <c r="K32" s="292"/>
       <c r="M32" s="19"/>
     </row>
-    <row r="33" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="210" t="s">
         <v>81</v>
       </c>
@@ -7380,15 +7397,15 @@
         <f>Sieblinie!C30</f>
         <v>11.5</v>
       </c>
-      <c r="I33" s="279" t="str">
+      <c r="I33" s="290" t="str">
         <f>Sieblinie!L15</f>
         <v>Okrilla</v>
       </c>
-      <c r="J33" s="280"/>
-      <c r="K33" s="281"/>
+      <c r="J33" s="291"/>
+      <c r="K33" s="292"/>
       <c r="M33" s="11"/>
     </row>
-    <row r="34" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="210" t="s">
         <v>83</v>
       </c>
@@ -7410,14 +7427,14 @@
         <f>Sieblinie!C31</f>
         <v>7.5</v>
       </c>
-      <c r="I34" s="279" t="str">
+      <c r="I34" s="290" t="str">
         <f>Sieblinie!L16</f>
         <v>Okrilla</v>
       </c>
-      <c r="J34" s="280"/>
-      <c r="K34" s="281"/>
-    </row>
-    <row r="35" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J34" s="291"/>
+      <c r="K34" s="292"/>
+    </row>
+    <row r="35" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="210" t="s">
         <v>131</v>
       </c>
@@ -7439,14 +7456,14 @@
         <f>Sieblinie!C32</f>
         <v>7.5</v>
       </c>
-      <c r="I35" s="279" t="str">
+      <c r="I35" s="290" t="str">
         <f>Sieblinie!L17</f>
         <v>Okrilla</v>
       </c>
-      <c r="J35" s="280"/>
-      <c r="K35" s="281"/>
-    </row>
-    <row r="36" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J35" s="291"/>
+      <c r="K35" s="292"/>
+    </row>
+    <row r="36" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="210" t="s">
         <v>120</v>
       </c>
@@ -7468,13 +7485,13 @@
         <f>Sieblinie!C33</f>
         <v>42</v>
       </c>
-      <c r="I36" s="279" t="s">
+      <c r="I36" s="290" t="s">
         <v>152</v>
       </c>
-      <c r="J36" s="280"/>
-      <c r="K36" s="281"/>
-    </row>
-    <row r="37" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J36" s="291"/>
+      <c r="K36" s="292"/>
+    </row>
+    <row r="37" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="210"/>
       <c r="B37" s="138"/>
       <c r="C37" s="214" t="s">
@@ -7491,12 +7508,12 @@
       <c r="H37" s="216" t="s">
         <v>88</v>
       </c>
-      <c r="I37" s="295"/>
-      <c r="J37" s="296"/>
-      <c r="K37" s="297"/>
+      <c r="I37" s="284"/>
+      <c r="J37" s="285"/>
+      <c r="K37" s="286"/>
       <c r="M37" s="19"/>
     </row>
-    <row r="38" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="79"/>
       <c r="B38" s="72"/>
       <c r="C38" s="217" t="s">
@@ -7513,12 +7530,12 @@
       <c r="H38" s="219" t="s">
         <v>88</v>
       </c>
-      <c r="I38" s="298"/>
-      <c r="J38" s="299"/>
-      <c r="K38" s="300"/>
+      <c r="I38" s="287"/>
+      <c r="J38" s="288"/>
+      <c r="K38" s="289"/>
       <c r="M38" s="11"/>
     </row>
-    <row r="39" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="70" t="s">
         <v>91</v>
       </c>
@@ -7537,11 +7554,11 @@
         <v>1000</v>
       </c>
       <c r="H39" s="85"/>
-      <c r="I39" s="298"/>
-      <c r="J39" s="299"/>
-      <c r="K39" s="300"/>
-    </row>
-    <row r="40" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I39" s="287"/>
+      <c r="J39" s="288"/>
+      <c r="K39" s="289"/>
+    </row>
+    <row r="40" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="70" t="s">
         <v>121</v>
       </c>
@@ -7558,11 +7575,11 @@
         <v>65</v>
       </c>
       <c r="H40" s="72"/>
-      <c r="I40" s="298"/>
-      <c r="J40" s="299"/>
-      <c r="K40" s="300"/>
-    </row>
-    <row r="41" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I40" s="287"/>
+      <c r="J40" s="288"/>
+      <c r="K40" s="289"/>
+    </row>
+    <row r="41" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="141" t="s">
         <v>122</v>
       </c>
@@ -7579,11 +7596,11 @@
         <v>65</v>
       </c>
       <c r="H41" s="45"/>
-      <c r="I41" s="292"/>
-      <c r="J41" s="293"/>
-      <c r="K41" s="294"/>
-    </row>
-    <row r="42" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I41" s="281"/>
+      <c r="J41" s="282"/>
+      <c r="K41" s="283"/>
+    </row>
+    <row r="42" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
@@ -7596,7 +7613,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -7609,7 +7626,7 @@
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
     </row>
-    <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="12"/>
@@ -7623,7 +7640,7 @@
       <c r="K44" s="6"/>
       <c r="L44" s="14"/>
     </row>
-    <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -7637,7 +7654,7 @@
       <c r="K45" s="6"/>
       <c r="L45" s="10"/>
     </row>
-    <row r="46" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46" s="16"/>
@@ -7651,7 +7668,7 @@
       <c r="K46" s="10"/>
       <c r="L46" s="16"/>
     </row>
-    <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="10"/>
       <c r="C47" s="12"/>
@@ -7665,15 +7682,21 @@
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
     </row>
-    <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="C48" s="17"/>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G51" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I30:K30"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="I41:K41"/>
     <mergeCell ref="I37:K37"/>
@@ -7690,12 +7713,6 @@
     <mergeCell ref="I25:K25"/>
     <mergeCell ref="I28:K28"/>
     <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I30:K30"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.62992125984251968" bottom="0" header="0.51181102362204722" footer="0.23622047244094491"/>
@@ -7707,31 +7724,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" customWidth="1"/>
-    <col min="6" max="6" width="1.140625" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" customWidth="1"/>
-    <col min="8" max="8" width="1.140625" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="3.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="1.109375" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" customWidth="1"/>
+    <col min="8" max="8" width="1.109375" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" customWidth="1"/>
     <col min="11" max="11" width="8" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" customWidth="1"/>
+    <col min="12" max="12" width="7.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="277" t="str">
+    <row r="1" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="279" t="str">
         <f>Rezeptur!A1</f>
         <v>BAM
 7.4</v>
@@ -7749,14 +7766,14 @@
       <c r="J1" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="301">
+      <c r="K1" s="303">
         <f>Sieblinie!L1</f>
         <v>43209</v>
       </c>
-      <c r="L1" s="302"/>
-    </row>
-    <row r="2" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="278"/>
+      <c r="L1" s="304"/>
+    </row>
+    <row r="2" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="280"/>
       <c r="B2" s="42" t="s">
         <v>43</v>
       </c>
@@ -7776,7 +7793,7 @@
       </c>
       <c r="L2" s="45"/>
     </row>
-    <row r="3" spans="1:12" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="46"/>
       <c r="C3" s="46"/>
@@ -7790,7 +7807,7 @@
       <c r="K3" s="46"/>
       <c r="L3" s="46"/>
     </row>
-    <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>4</v>
       </c>
@@ -7811,7 +7828,7 @@
       <c r="K4" s="49"/>
       <c r="L4" s="49"/>
     </row>
-    <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>5</v>
       </c>
@@ -7833,7 +7850,7 @@
       </c>
       <c r="L5" s="49"/>
     </row>
-    <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>45</v>
       </c>
@@ -7854,7 +7871,7 @@
       <c r="K6" s="49"/>
       <c r="L6" s="49"/>
     </row>
-    <row r="7" spans="1:12" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47"/>
       <c r="B7" s="47"/>
       <c r="C7" s="47"/>
@@ -7868,7 +7885,7 @@
       <c r="K7" s="47"/>
       <c r="L7" s="47"/>
     </row>
-    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
         <v>46</v>
       </c>
@@ -7886,7 +7903,7 @@
       <c r="K8" s="53"/>
       <c r="L8" s="52"/>
     </row>
-    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
         <v>48</v>
       </c>
@@ -7908,7 +7925,7 @@
       <c r="K9" s="58"/>
       <c r="L9" s="59"/>
     </row>
-    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="60"/>
       <c r="B10" s="61"/>
       <c r="C10" s="62" t="s">
@@ -7936,7 +7953,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="70"/>
       <c r="B11" s="66"/>
       <c r="C11" s="71"/>
@@ -7953,12 +7970,12 @@
         <v>167</v>
       </c>
       <c r="J11" s="67"/>
-      <c r="K11" s="314" t="s">
+      <c r="K11" s="277" t="s">
         <v>166</v>
       </c>
       <c r="L11" s="69"/>
     </row>
-    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="77" t="s">
         <v>57</v>
       </c>
@@ -7984,7 +8001,7 @@
       <c r="K12" s="76"/>
       <c r="L12" s="69"/>
     </row>
-    <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="70" t="s">
         <v>61</v>
       </c>
@@ -8013,7 +8030,7 @@
       <c r="K13" s="68"/>
       <c r="L13" s="69"/>
     </row>
-    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="70" t="s">
         <v>62</v>
       </c>
@@ -8037,12 +8054,12 @@
         <v>63</v>
       </c>
       <c r="J14" s="88"/>
-      <c r="K14" s="315">
+      <c r="K14" s="278">
         <v>0.7</v>
       </c>
       <c r="L14" s="89"/>
     </row>
-    <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="70" t="s">
         <v>64</v>
       </c>
@@ -8066,7 +8083,7 @@
       <c r="K15" s="92"/>
       <c r="L15" s="66"/>
     </row>
-    <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="70" t="s">
         <v>67</v>
       </c>
@@ -8092,7 +8109,7 @@
       </c>
       <c r="L16" s="69"/>
     </row>
-    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="70" t="s">
         <v>69</v>
       </c>
@@ -8124,7 +8141,7 @@
       </c>
       <c r="L17" s="69"/>
     </row>
-    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="70" t="s">
         <v>147</v>
       </c>
@@ -8157,7 +8174,7 @@
       </c>
       <c r="L18" s="102"/>
     </row>
-    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="70" t="s">
         <v>71</v>
       </c>
@@ -8181,7 +8198,7 @@
       <c r="K19" s="92"/>
       <c r="L19" s="66"/>
     </row>
-    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="104" t="s">
         <v>73</v>
       </c>
@@ -8212,7 +8229,7 @@
       </c>
       <c r="L20" s="114"/>
     </row>
-    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="115" t="s">
         <v>76</v>
       </c>
@@ -8245,7 +8262,7 @@
       <c r="K21" s="119"/>
       <c r="L21" s="120"/>
     </row>
-    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="115" t="s">
         <v>77</v>
       </c>
@@ -8278,7 +8295,7 @@
       <c r="K22" s="92"/>
       <c r="L22" s="66"/>
     </row>
-    <row r="23" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="115" t="s">
         <v>79</v>
       </c>
@@ -8314,7 +8331,7 @@
       </c>
       <c r="L23" s="124"/>
     </row>
-    <row r="24" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="115" t="s">
         <v>81</v>
       </c>
@@ -8347,7 +8364,7 @@
       <c r="K24" s="99"/>
       <c r="L24" s="120"/>
     </row>
-    <row r="25" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="115" t="s">
         <v>83</v>
       </c>
@@ -8380,7 +8397,7 @@
       <c r="K25" s="127"/>
       <c r="L25" s="66"/>
     </row>
-    <row r="26" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="115" t="s">
         <v>85</v>
       </c>
@@ -8411,7 +8428,7 @@
       <c r="K26" s="83"/>
       <c r="L26" s="131"/>
     </row>
-    <row r="27" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="115" t="s">
         <v>86</v>
       </c>
@@ -8442,7 +8459,7 @@
       <c r="K27" s="133"/>
       <c r="L27" s="124"/>
     </row>
-    <row r="28" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="115" t="s">
         <v>87</v>
       </c>
@@ -8466,7 +8483,7 @@
       <c r="K28" s="99"/>
       <c r="L28" s="120"/>
     </row>
-    <row r="29" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="137" t="s">
         <v>65</v>
       </c>
@@ -8492,7 +8509,7 @@
       <c r="K29" s="92"/>
       <c r="L29" s="66"/>
     </row>
-    <row r="30" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="90" t="s">
         <v>65</v>
       </c>
@@ -8520,7 +8537,7 @@
       </c>
       <c r="L30" s="124"/>
     </row>
-    <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="141" t="s">
         <v>91</v>
       </c>
@@ -8547,7 +8564,7 @@
       <c r="K31" s="99"/>
       <c r="L31" s="120"/>
     </row>
-    <row r="32" spans="1:12" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="148"/>
       <c r="B32" s="148"/>
       <c r="C32" s="149"/>
@@ -8561,7 +8578,7 @@
       <c r="K32" s="48"/>
       <c r="L32" s="48"/>
     </row>
-    <row r="33" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="50" t="s">
         <v>92</v>
       </c>
@@ -8573,16 +8590,16 @@
       </c>
       <c r="F33" s="152"/>
       <c r="G33" s="152"/>
-      <c r="H33" s="309">
+      <c r="H33" s="311">
         <f>K1</f>
         <v>43209</v>
       </c>
-      <c r="I33" s="309"/>
-      <c r="J33" s="309"/>
+      <c r="I33" s="311"/>
+      <c r="J33" s="311"/>
       <c r="K33" s="152"/>
       <c r="L33" s="153"/>
     </row>
-    <row r="34" spans="1:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="154" t="s">
         <v>94</v>
       </c>
@@ -8591,16 +8608,16 @@
         <v>95</v>
       </c>
       <c r="D34" s="157"/>
-      <c r="E34" s="312"/>
-      <c r="F34" s="313"/>
-      <c r="G34" s="312"/>
-      <c r="H34" s="313"/>
+      <c r="E34" s="314"/>
+      <c r="F34" s="315"/>
+      <c r="G34" s="314"/>
+      <c r="H34" s="315"/>
       <c r="I34" s="33"/>
       <c r="J34" s="33"/>
       <c r="K34" s="33"/>
       <c r="L34" s="34"/>
     </row>
-    <row r="35" spans="1:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="158" t="s">
         <v>96</v>
       </c>
@@ -8609,14 +8626,14 @@
         <v>59</v>
       </c>
       <c r="D35" s="160"/>
-      <c r="E35" s="310">
+      <c r="E35" s="312">
         <v>7829</v>
       </c>
-      <c r="F35" s="311"/>
-      <c r="G35" s="310">
+      <c r="F35" s="313"/>
+      <c r="G35" s="312">
         <v>7891</v>
       </c>
-      <c r="H35" s="311"/>
+      <c r="H35" s="313"/>
       <c r="I35" s="95">
         <v>7959</v>
       </c>
@@ -8630,7 +8647,7 @@
         <v>7875</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="158" t="s">
         <v>97</v>
       </c>
@@ -8650,7 +8667,7 @@
       <c r="K36" s="113"/>
       <c r="L36" s="114"/>
     </row>
-    <row r="37" spans="1:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="161" t="s">
         <v>99</v>
       </c>
@@ -8659,16 +8676,16 @@
         <v>100</v>
       </c>
       <c r="D37" s="164"/>
-      <c r="E37" s="303">
+      <c r="E37" s="305">
         <f>ROUND(E35/E36,-1)</f>
         <v>2320</v>
       </c>
-      <c r="F37" s="304"/>
-      <c r="G37" s="303">
+      <c r="F37" s="306"/>
+      <c r="G37" s="305">
         <f>ROUND(G35/E36,-1)</f>
         <v>2340</v>
       </c>
-      <c r="H37" s="304"/>
+      <c r="H37" s="306"/>
       <c r="I37" s="165">
         <f>ROUND(I35/E36,-1)</f>
         <v>2360</v>
@@ -8686,7 +8703,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="167" t="s">
         <v>101</v>
       </c>
@@ -8695,22 +8712,22 @@
         <v>100</v>
       </c>
       <c r="D38" s="169"/>
-      <c r="E38" s="305">
+      <c r="E38" s="307">
         <f>ROUND(AVERAGE(E37:I37),-1)</f>
         <v>2340</v>
       </c>
-      <c r="F38" s="306"/>
-      <c r="G38" s="306"/>
-      <c r="H38" s="306"/>
-      <c r="I38" s="307"/>
-      <c r="J38" s="305">
+      <c r="F38" s="308"/>
+      <c r="G38" s="308"/>
+      <c r="H38" s="308"/>
+      <c r="I38" s="309"/>
+      <c r="J38" s="307">
         <f>ROUND(AVERAGE(J37:L37),-1)</f>
         <v>2350</v>
       </c>
-      <c r="K38" s="306"/>
-      <c r="L38" s="308"/>
-    </row>
-    <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K38" s="308"/>
+      <c r="L38" s="310"/>
+    </row>
+    <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="266" t="s">
         <v>160</v>
       </c>
@@ -8730,7 +8747,7 @@
       <c r="K39" s="266"/>
       <c r="L39" s="266"/>
     </row>
-    <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="266" t="s">
         <v>161</v>
       </c>
@@ -8750,7 +8767,7 @@
       <c r="K40" s="266"/>
       <c r="L40" s="266"/>
     </row>
-    <row r="41" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="272" t="s">
         <v>162</v>
       </c>
@@ -8770,7 +8787,7 @@
       <c r="K41" s="266"/>
       <c r="L41" s="266"/>
     </row>
-    <row r="42" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="272" t="s">
         <v>163</v>
       </c>
@@ -8790,7 +8807,7 @@
       <c r="K42" s="269"/>
       <c r="L42" s="269"/>
     </row>
-    <row r="43" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="274"/>
       <c r="B43" s="274"/>
       <c r="C43" s="274"/>
@@ -8808,7 +8825,7 @@
       <c r="K43" s="274"/>
       <c r="L43" s="274"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="48"/>
       <c r="B44" s="48"/>
       <c r="C44" s="48"/>
@@ -8822,7 +8839,7 @@
       <c r="K44" s="48"/>
       <c r="L44" s="48"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="48"/>
       <c r="B45" s="48"/>
       <c r="C45" s="48"/>

</xml_diff>